<commit_message>
Updated CPU time tracking tables.
For simplicity and ease of maintenance, deleted "documents/CPU_timing/mSigHdp-paper-tracking-CPU-time-only.xlsx"
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/cpu-simpler.xlsx
+++ b/documents/CPU_timing/cpu-simpler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D405EE-7533-4387-B9C9-EFA6D7A8BF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC9CEA2-A79C-441B-BD2C-E20F3B08B794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="2985" windowWidth="17100" windowHeight="12855" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11535" yWindow="345" windowWidth="17100" windowHeight="12855" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>2.45 (3.5)</t>
+  </si>
+  <si>
+    <t>Finished re-running</t>
   </si>
 </sst>
 </file>
@@ -278,7 +281,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -351,6 +354,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -812,7 +818,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -901,11 +907,11 @@
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E5" s="19"/>
       <c r="F5" s="23" t="s">
@@ -949,11 +955,11 @@
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E8" s="19"/>
       <c r="F8" s="23" t="s">
@@ -1036,11 +1042,11 @@
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="25" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="23" t="s">
@@ -1072,7 +1078,7 @@
       </c>
       <c r="J14" s="14"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" hidden="1">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1082,7 +1088,9 @@
       <c r="C15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="19" t="s">
+        <v>44</v>
+      </c>
       <c r="E15" s="19"/>
       <c r="F15" s="23" t="s">
         <v>43</v>
@@ -1108,7 +1116,7 @@
       </c>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" spans="1:10" s="9" customFormat="1">
+    <row r="17" spans="1:10" s="9" customFormat="1" hidden="1">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -1164,7 +1172,7 @@
       </c>
       <c r="J19" s="14"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" hidden="1">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
@@ -1203,7 +1211,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" hidden="1">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
@@ -1257,7 +1265,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" hidden="1">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
@@ -1273,7 +1281,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" hidden="1">
       <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
@@ -1287,7 +1295,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" hidden="1">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1336,6 +1344,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H27" xr:uid="{81A9EF94-C3F0-491E-B97E-7A2B5FFF7AB0}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="indel_set1"/>
+        <filter val="indel_set2"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="2">
       <filters>
         <filter val="HPC"/>

</xml_diff>

<commit_message>
Updated CPU info and timing tables.
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/cpu-simpler.xlsx
+++ b/documents/CPU_timing/cpu-simpler.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC9CEA2-A79C-441B-BD2C-E20F3B08B794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09283BAE-49D7-4B83-B80D-75F7D1E00000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11535" yWindow="345" windowWidth="17100" windowHeight="12855" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10590" yWindow="1590" windowWidth="18015" windowHeight="12855" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
     <sheet name="Combined" sheetId="10" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Combined!$A$1:$H$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Combined!$A$1:$F$27</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="45">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -149,9 +149,6 @@
     <t>monster2</t>
   </si>
   <si>
-    <t>re-run on HPC</t>
-  </si>
-  <si>
     <t>2) Texts highlighted in red stands for machine other than HPC</t>
   </si>
   <si>
@@ -178,7 +175,23 @@
     <t>2.45 (3.5)</t>
   </si>
   <si>
-    <t>Finished re-running</t>
+    <t>AMD EPYC 7763</t>
+  </si>
+  <si>
+    <r>
+      <t>HPC/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>monster2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -241,18 +254,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -281,7 +288,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -310,37 +317,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -354,9 +355,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -784,10 +782,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -812,13 +810,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A9EF94-C3F0-491E-B97E-7A2B5FFF7AB0}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -826,13 +824,12 @@
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="22"/>
-    <col min="5" max="5" width="14.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="22" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="20"/>
+    <col min="5" max="5" width="14.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" customHeight="1">
+    <row r="1" spans="1:8" ht="45" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
@@ -846,474 +843,492 @@
         <v>30</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="C2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="E3" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="E4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="C5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="C6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="C7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="C8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="E9" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="E10" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="C11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="J12" s="14"/>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="C12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="1:10" hidden="1">
-      <c r="A14" s="22" t="s">
+      <c r="C13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:10" hidden="1">
+      <c r="E14" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="19" t="s">
+      <c r="C15" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" s="14"/>
-    </row>
-    <row r="16" spans="1:10" hidden="1">
+      <c r="D15" s="17"/>
+      <c r="E15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" s="14"/>
-    </row>
-    <row r="17" spans="1:10" s="9" customFormat="1" hidden="1">
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" s="9" customFormat="1">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="1:10" hidden="1">
+      <c r="E17" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19" t="s">
+      <c r="D18" s="17"/>
+      <c r="E18" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="14"/>
-    </row>
-    <row r="19" spans="1:10" hidden="1">
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="1:10" hidden="1">
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="19"/>
-      <c r="F20" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" hidden="1">
+      <c r="C20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" hidden="1">
+      <c r="D21" s="17"/>
+      <c r="E21" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1">
+      <c r="C22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" hidden="1">
+      <c r="E23" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" hidden="1">
+      <c r="C25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" hidden="1">
+      <c r="C26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="19" t="s">
+      <c r="C27" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="19"/>
-      <c r="F27" s="23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="E27" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1321,47 +1336,36 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="98.1" customHeight="1">
-      <c r="A29" s="24" t="s">
+    <row r="29" spans="1:8" ht="60" customHeight="1">
+      <c r="A29" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:8">
       <c r="A31" s="5" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H27" xr:uid="{81A9EF94-C3F0-491E-B97E-7A2B5FFF7AB0}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="indel_set1"/>
-        <filter val="indel_set2"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="HPC"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H27">
+  <autoFilter ref="A1:F27" xr:uid="{81A9EF94-C3F0-491E-B97E-7A2B5FFF7AB0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F27">
       <sortCondition ref="B2:B27"/>
       <sortCondition ref="A2:A27"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Deleted lines for NR_hdp in cpu_simpler.xlsx
Also deleted redundant documents/lscpu_info.xlsx. Now these info are in
- documents/CPU_timing/hpc_cluster.cpuinfo
- documents/CPU_timing/minimonster.cpuinfo
- documents/CPU_timing/monster2.cpuinfo
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/cpu-simpler.xlsx
+++ b/documents/CPU_timing/cpu-simpler.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rozen\Documents\GitHub\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ABCB46-8480-4E8B-81B4-EA9D907F106E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F3484F-6C5B-4134-86BE-265E8240DEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="82020" yWindow="-11370" windowWidth="32940" windowHeight="18795" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3255" yWindow="2070" windowWidth="18015" windowHeight="12855" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
     <sheet name="Combined" sheetId="10" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Combined!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Combined!$A$1:$F$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="46">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -95,16 +95,7 @@
     <t>hdp-NR()</t>
   </si>
   <si>
-    <t>NR_hdp_gb_1</t>
-  </si>
-  <si>
-    <t>NR_hdp_gb_20</t>
-  </si>
-  <si>
     <t>3) Here, "gb" stands for the value of "gamma.beta" used to run R package `hdp` by Nicola D Roberts</t>
-  </si>
-  <si>
-    <t>NR_hdp_gb_50</t>
   </si>
   <si>
     <t>Data set name</t>
@@ -210,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,31 +256,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -325,7 +291,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -351,9 +317,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -369,9 +332,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -387,38 +347,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="2" xr:uid="{4DBD74BB-9B12-4298-9AA6-0A807FEE0790}"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -710,7 +646,7 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
@@ -723,7 +659,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="43.5">
+    <row r="2" spans="1:6" ht="45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -840,10 +776,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -871,20 +807,20 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
-    <col min="3" max="3" width="28.81640625" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="19"/>
-    <col min="5" max="5" width="14.54296875" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="17"/>
+    <col min="5" max="5" width="14.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="45" customHeight="1">
@@ -892,19 +828,19 @@
         <v>4</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -912,533 +848,385 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>42</v>
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>42</v>
+      <c r="E3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>42</v>
+      <c r="E4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>42</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>42</v>
+        <v>23</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>42</v>
+        <v>23</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>42</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="20" t="s">
+      <c r="C10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>42</v>
-      </c>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>42</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="13"/>
+      <c r="C12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="12"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="11" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="13"/>
+      <c r="C14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="14"/>
       <c r="E15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="60" customHeight="1">
+      <c r="A21" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="1:8" s="9" customFormat="1">
-      <c r="A17" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" ht="60" customHeight="1">
-      <c r="A29" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="5" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F27" xr:uid="{81A9EF94-C3F0-491E-B97E-7A2B5FFF7AB0}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F27">
-      <sortCondition ref="B2:B27"/>
-      <sortCondition ref="A2:A27"/>
+  <autoFilter ref="A1:F19" xr:uid="{81A9EF94-C3F0-491E-B97E-7A2B5FFF7AB0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
+      <sortCondition ref="B2:B19"/>
+      <sortCondition ref="A2:A19"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">
-    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated CPU timing tables:
* cpu-simpler.xlsx
* mSigHdp-paper-tracking.xlsx
</commit_message>
<xml_diff>
--- a/documents/CPU_timing/cpu-simpler.xlsx
+++ b/documents/CPU_timing/cpu-simpler.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\documents\CPU_timing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F3484F-6C5B-4134-86BE-265E8240DEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2E9E99-946D-484C-9251-5AF2306D8999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3255" yWindow="2070" windowWidth="18015" windowHeight="12855" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2475" yWindow="2670" windowWidth="15615" windowHeight="12045" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="45">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -137,9 +137,6 @@
     <t>minimonster</t>
   </si>
   <si>
-    <t>monster2</t>
-  </si>
-  <si>
     <t>2) Texts highlighted in red stands for machine other than HPC</t>
   </si>
   <si>
@@ -169,39 +166,26 @@
     <t>AMD EPYC 7763</t>
   </si>
   <si>
-    <r>
-      <t>HPC/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>monster2</t>
-    </r>
-  </si>
-  <si>
     <t>rerun on HPC</t>
   </si>
   <si>
     <t>maybe rerun on HPC</t>
   </si>
   <si>
-    <t>why both HPC and monster2?</t>
-  </si>
-  <si>
-    <t>low priority re-run on HPC</t>
+    <t>Previously on monster2</t>
+  </si>
+  <si>
+    <t>re-running on HPC</t>
+  </si>
+  <si>
+    <t>Finished on both monster2 and HPC, yet having different results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +240,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -291,7 +284,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -349,6 +342,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -810,7 +807,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -818,7 +815,7 @@
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="17"/>
+    <col min="4" max="4" width="17.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" style="17" customWidth="1"/>
   </cols>
@@ -837,10 +834,10 @@
         <v>27</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -855,10 +852,10 @@
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -873,10 +870,10 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -890,10 +887,10 @@
         <v>21</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -908,10 +905,10 @@
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -926,10 +923,10 @@
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -944,10 +941,10 @@
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -962,10 +959,10 @@
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="12"/>
     </row>
@@ -981,10 +978,10 @@
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9" s="12"/>
     </row>
@@ -1002,13 +999,13 @@
         <v>28</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H10" s="12"/>
     </row>
@@ -1020,18 +1017,16 @@
         <v>24</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>44</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="G11" s="14"/>
       <c r="H11" s="12"/>
     </row>
     <row r="12" spans="1:8">
@@ -1041,18 +1036,20 @@
       <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="14"/>
+      <c r="C12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="E12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H12" s="12"/>
     </row>
@@ -1063,17 +1060,17 @@
       <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>31</v>
+      <c r="C13" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="E13" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" t="s">
-        <v>45</v>
+      <c r="G13" s="20" t="s">
+        <v>44</v>
       </c>
       <c r="H13" s="12"/>
     </row>
@@ -1089,10 +1086,10 @@
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1107,13 +1104,13 @@
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1128,10 +1125,10 @@
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1146,10 +1143,10 @@
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1163,10 +1160,10 @@
         <v>21</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1176,17 +1173,15 @@
       <c r="B19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>28</v>
-      </c>
+      <c r="C19" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="14"/>
       <c r="E19" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1209,7 +1204,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="5"/>
     </row>

</xml_diff>